<commit_message>
pictures instead of letters
</commit_message>
<xml_diff>
--- a/hiragana1.xlsx
+++ b/hiragana1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mt00212\Documents\Tasks\Probabilistic Learning\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\uni\PhD\Tasks\Probabilistic Learning Pavlovia\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -20,9 +20,6 @@
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="14">
-  <si>
-    <t>A</t>
-  </si>
   <si>
     <t>letter1</t>
   </si>
@@ -39,18 +36,6 @@
     <t>c</t>
   </si>
   <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>O</t>
-  </si>
-  <si>
-    <t>d</t>
-  </si>
-  <si>
-    <t>I</t>
-  </si>
-  <si>
     <t>letterA</t>
   </si>
   <si>
@@ -60,14 +45,29 @@
     <t>letterE</t>
   </si>
   <si>
-    <t>L</t>
+    <t>1.jpg</t>
+  </si>
+  <si>
+    <t>2.jpg</t>
+  </si>
+  <si>
+    <t>3.jpg</t>
+  </si>
+  <si>
+    <t>4.jpg</t>
+  </si>
+  <si>
+    <t>5.jpg</t>
+  </si>
+  <si>
+    <t>6.jpg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="21" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="22">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -217,6 +217,11 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri "/>
     </font>
   </fonts>
   <fills count="33">
@@ -560,11 +565,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -888,11 +894,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H91"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30:A31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="21.28515625" customWidth="1"/>
     <col min="2" max="2" width="19.140625" customWidth="1"/>
@@ -909,762 +915,762 @@
     <col min="16" max="16" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
-        <v>3</v>
-      </c>
       <c r="D1" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E1" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="F1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="78.75" x14ac:dyDescent="1.05">
-      <c r="A2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="78.75">
+      <c r="A2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G2" s="2"/>
       <c r="H2" s="2"/>
     </row>
-    <row r="3" spans="1:8" ht="78.75" x14ac:dyDescent="1.05">
-      <c r="A3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>6</v>
+    <row r="3" spans="1:8" ht="78.75">
+      <c r="A3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G3" s="2"/>
       <c r="H3" s="2"/>
     </row>
-    <row r="4" spans="1:8" ht="78.75" x14ac:dyDescent="1.05">
-      <c r="A4" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>6</v>
+    <row r="4" spans="1:8" ht="78.75">
+      <c r="A4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
     </row>
-    <row r="5" spans="1:8" ht="78.75" x14ac:dyDescent="1.05">
-      <c r="A5" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>6</v>
+    <row r="5" spans="1:8" ht="78.75">
+      <c r="A5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:8" ht="78.75" x14ac:dyDescent="1.05">
-      <c r="A6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>0</v>
+    <row r="6" spans="1:8" ht="78.75">
+      <c r="A6" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>8</v>
       </c>
       <c r="C6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
     </row>
-    <row r="7" spans="1:8" ht="78.75" x14ac:dyDescent="1.05">
-      <c r="A7" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>0</v>
+    <row r="7" spans="1:8" ht="78.75">
+      <c r="A7" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
     </row>
-    <row r="8" spans="1:8" ht="78.75" x14ac:dyDescent="1.05">
-      <c r="A8" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>0</v>
+    <row r="8" spans="1:8" ht="78.75">
+      <c r="A8" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D8" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
     </row>
-    <row r="9" spans="1:8" ht="78.75" x14ac:dyDescent="1.05">
-      <c r="A9" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>0</v>
+    <row r="9" spans="1:8" ht="78.75">
+      <c r="A9" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:8" ht="78.75" x14ac:dyDescent="1.05">
-      <c r="A10" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>6</v>
+    <row r="10" spans="1:8" ht="78.75">
+      <c r="A10" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
     </row>
-    <row r="11" spans="1:8" ht="78.75" x14ac:dyDescent="1.05">
-      <c r="A11" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>0</v>
+    <row r="11" spans="1:8" ht="78.75">
+      <c r="A11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>8</v>
       </c>
       <c r="C11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
     </row>
-    <row r="12" spans="1:8" ht="78.75" x14ac:dyDescent="1.05">
-      <c r="A12" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>8</v>
+    <row r="12" spans="1:8" ht="78.75">
+      <c r="A12" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="1:8" ht="78.75" x14ac:dyDescent="1.05">
-      <c r="A13" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>8</v>
+    <row r="13" spans="1:8" ht="78.75">
+      <c r="A13" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
     </row>
-    <row r="14" spans="1:8" ht="78.75" x14ac:dyDescent="1.05">
-      <c r="A14" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>8</v>
+    <row r="14" spans="1:8" ht="78.75">
+      <c r="A14" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="C14" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G14" s="2"/>
       <c r="H14" s="2"/>
     </row>
-    <row r="15" spans="1:8" ht="78.75" x14ac:dyDescent="1.05">
-      <c r="A15" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>8</v>
+    <row r="15" spans="1:8" ht="78.75">
+      <c r="A15" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="C15" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D15" s="1"/>
       <c r="E15" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
     </row>
-    <row r="16" spans="1:8" ht="78.75" x14ac:dyDescent="1.05">
-      <c r="A16" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>7</v>
+    <row r="16" spans="1:8" ht="78.75">
+      <c r="A16" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>10</v>
       </c>
       <c r="C16" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D16" s="1"/>
       <c r="E16" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
     </row>
-    <row r="17" spans="1:8" ht="78.75" x14ac:dyDescent="1.05">
-      <c r="A17" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>7</v>
+    <row r="17" spans="1:8" ht="78.75">
+      <c r="A17" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>10</v>
       </c>
       <c r="C17" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
     </row>
-    <row r="18" spans="1:8" ht="78.75" x14ac:dyDescent="1.05">
-      <c r="A18" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>7</v>
+    <row r="18" spans="1:8" ht="78.75">
+      <c r="A18" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>10</v>
       </c>
       <c r="C18" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D18" s="1"/>
       <c r="E18" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
     </row>
-    <row r="19" spans="1:8" ht="78.75" x14ac:dyDescent="1.05">
-      <c r="A19" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>7</v>
+    <row r="19" spans="1:8" ht="78.75">
+      <c r="A19" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>10</v>
       </c>
       <c r="C19" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
     </row>
-    <row r="20" spans="1:8" ht="78.75" x14ac:dyDescent="1.05">
-      <c r="A20" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>7</v>
+    <row r="20" spans="1:8" ht="78.75">
+      <c r="A20" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>10</v>
       </c>
       <c r="C20" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D20" s="1"/>
       <c r="E20" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
     </row>
-    <row r="21" spans="1:8" ht="78.75" x14ac:dyDescent="1.05">
-      <c r="A21" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>8</v>
+    <row r="21" spans="1:8" ht="78.75">
+      <c r="A21" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>11</v>
       </c>
       <c r="C21" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E21" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
     </row>
-    <row r="22" spans="1:8" ht="78.75" x14ac:dyDescent="1.05">
-      <c r="A22" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B22" s="2" t="s">
+    <row r="22" spans="1:8" ht="78.75">
+      <c r="A22" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B22" s="4" t="s">
         <v>13</v>
       </c>
       <c r="C22" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D22" s="1"/>
       <c r="F22" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
     </row>
-    <row r="23" spans="1:8" ht="78.75" x14ac:dyDescent="1.05">
-      <c r="A23" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B23" s="2" t="s">
+    <row r="23" spans="1:8" ht="78.75">
+      <c r="A23" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B23" s="4" t="s">
         <v>13</v>
       </c>
       <c r="C23" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D23" s="1"/>
       <c r="F23" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G23" s="2"/>
       <c r="H23" s="2"/>
     </row>
-    <row r="24" spans="1:8" ht="78.75" x14ac:dyDescent="1.05">
-      <c r="A24" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B24" s="2" t="s">
+    <row r="24" spans="1:8" ht="78.75">
+      <c r="A24" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B24" s="4" t="s">
         <v>13</v>
       </c>
       <c r="C24" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D24" s="1"/>
       <c r="F24" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
     </row>
-    <row r="25" spans="1:8" ht="78.75" x14ac:dyDescent="1.05">
-      <c r="A25" s="2" t="s">
+    <row r="25" spans="1:8" ht="78.75">
+      <c r="A25" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B25" s="2" t="s">
-        <v>9</v>
+      <c r="B25" s="4" t="s">
+        <v>12</v>
       </c>
       <c r="C25" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D25" s="1"/>
       <c r="F25" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
     </row>
-    <row r="26" spans="1:8" ht="78.75" x14ac:dyDescent="1.05">
-      <c r="A26" s="2" t="s">
+    <row r="26" spans="1:8" ht="78.75">
+      <c r="A26" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B26" s="2" t="s">
-        <v>9</v>
+      <c r="B26" s="4" t="s">
+        <v>12</v>
       </c>
       <c r="C26" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D26" s="1"/>
       <c r="F26" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
     </row>
-    <row r="27" spans="1:8" ht="78.75" x14ac:dyDescent="1.05">
-      <c r="A27" s="2" t="s">
+    <row r="27" spans="1:8" ht="78.75">
+      <c r="A27" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B27" s="2" t="s">
-        <v>9</v>
+      <c r="B27" s="4" t="s">
+        <v>12</v>
       </c>
       <c r="C27" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D27" s="1"/>
       <c r="F27" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
     </row>
-    <row r="28" spans="1:8" ht="78.75" x14ac:dyDescent="1.05">
-      <c r="A28" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B28" s="2" t="s">
+    <row r="28" spans="1:8" ht="78.75">
+      <c r="A28" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B28" s="4" t="s">
         <v>13</v>
       </c>
       <c r="C28" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D28" s="1"/>
       <c r="F28" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
     </row>
-    <row r="29" spans="1:8" ht="78.75" x14ac:dyDescent="1.05">
-      <c r="A29" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B29" s="2" t="s">
+    <row r="29" spans="1:8" ht="78.75">
+      <c r="A29" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B29" s="4" t="s">
         <v>13</v>
       </c>
       <c r="C29" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D29" s="1"/>
       <c r="F29" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
     </row>
-    <row r="30" spans="1:8" ht="78.75" x14ac:dyDescent="1.05">
-      <c r="A30" s="2" t="s">
+    <row r="30" spans="1:8" ht="78.75">
+      <c r="A30" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B30" s="2" t="s">
-        <v>9</v>
+      <c r="B30" s="4" t="s">
+        <v>12</v>
       </c>
       <c r="C30" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D30" s="1"/>
       <c r="F30" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
     </row>
-    <row r="31" spans="1:8" ht="78.75" x14ac:dyDescent="1.05">
-      <c r="A31" s="2" t="s">
+    <row r="31" spans="1:8" ht="78.75">
+      <c r="A31" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B31" s="2" t="s">
-        <v>9</v>
+      <c r="B31" s="4" t="s">
+        <v>12</v>
       </c>
       <c r="C31" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D31" s="1"/>
       <c r="F31" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
     </row>
-    <row r="32" spans="1:8" ht="78.75" x14ac:dyDescent="1.05">
+    <row r="32" spans="1:8" ht="78.75">
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
     </row>
-    <row r="33" spans="7:8" ht="78.75" x14ac:dyDescent="1.05">
+    <row r="33" spans="7:8" ht="78.75">
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
     </row>
-    <row r="34" spans="7:8" ht="78.75" x14ac:dyDescent="1.05">
+    <row r="34" spans="7:8" ht="78.75">
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
     </row>
-    <row r="35" spans="7:8" ht="78.75" x14ac:dyDescent="1.05">
+    <row r="35" spans="7:8" ht="78.75">
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
     </row>
-    <row r="36" spans="7:8" ht="78.75" x14ac:dyDescent="1.05">
+    <row r="36" spans="7:8" ht="78.75">
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
     </row>
-    <row r="37" spans="7:8" ht="78.75" x14ac:dyDescent="1.05">
+    <row r="37" spans="7:8" ht="78.75">
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
     </row>
-    <row r="38" spans="7:8" ht="78.75" x14ac:dyDescent="1.05">
+    <row r="38" spans="7:8" ht="78.75">
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
     </row>
-    <row r="39" spans="7:8" ht="78.75" x14ac:dyDescent="1.05">
+    <row r="39" spans="7:8" ht="78.75">
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
     </row>
-    <row r="40" spans="7:8" ht="78.75" x14ac:dyDescent="1.05">
+    <row r="40" spans="7:8" ht="78.75">
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
     </row>
-    <row r="41" spans="7:8" ht="78.75" x14ac:dyDescent="1.05">
+    <row r="41" spans="7:8" ht="78.75">
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
     </row>
-    <row r="42" spans="7:8" ht="78.75" x14ac:dyDescent="1.05">
+    <row r="42" spans="7:8" ht="78.75">
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
     </row>
-    <row r="43" spans="7:8" ht="78.75" x14ac:dyDescent="1.05">
+    <row r="43" spans="7:8" ht="78.75">
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
     </row>
-    <row r="44" spans="7:8" ht="78.75" x14ac:dyDescent="1.05">
+    <row r="44" spans="7:8" ht="78.75">
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
     </row>
-    <row r="45" spans="7:8" ht="78.75" x14ac:dyDescent="1.05">
+    <row r="45" spans="7:8" ht="78.75">
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
     </row>
-    <row r="46" spans="7:8" ht="78.75" x14ac:dyDescent="1.05">
+    <row r="46" spans="7:8" ht="78.75">
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
     </row>
-    <row r="47" spans="7:8" ht="78.75" x14ac:dyDescent="1.05">
+    <row r="47" spans="7:8" ht="78.75">
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
     </row>
-    <row r="48" spans="7:8" ht="78.75" x14ac:dyDescent="1.05">
+    <row r="48" spans="7:8" ht="78.75">
       <c r="G48" s="2"/>
       <c r="H48" s="2"/>
     </row>
-    <row r="49" spans="7:8" ht="78.75" x14ac:dyDescent="1.05">
+    <row r="49" spans="7:8" ht="78.75">
       <c r="G49" s="2"/>
       <c r="H49" s="2"/>
     </row>
-    <row r="50" spans="7:8" ht="78.75" x14ac:dyDescent="1.05">
+    <row r="50" spans="7:8" ht="78.75">
       <c r="G50" s="2"/>
       <c r="H50" s="2"/>
     </row>
-    <row r="51" spans="7:8" ht="78.75" x14ac:dyDescent="1.05">
+    <row r="51" spans="7:8" ht="78.75">
       <c r="G51" s="2"/>
       <c r="H51" s="2"/>
     </row>
-    <row r="52" spans="7:8" ht="78.75" x14ac:dyDescent="1.05">
+    <row r="52" spans="7:8" ht="78.75">
       <c r="G52" s="2"/>
       <c r="H52" s="2"/>
     </row>
-    <row r="53" spans="7:8" ht="78.75" x14ac:dyDescent="1.05">
+    <row r="53" spans="7:8" ht="78.75">
       <c r="G53" s="2"/>
       <c r="H53" s="2"/>
     </row>
-    <row r="54" spans="7:8" ht="78.75" x14ac:dyDescent="1.05">
+    <row r="54" spans="7:8" ht="78.75">
       <c r="G54" s="2"/>
       <c r="H54" s="2"/>
     </row>
-    <row r="55" spans="7:8" ht="78.75" x14ac:dyDescent="1.05">
+    <row r="55" spans="7:8" ht="78.75">
       <c r="G55" s="2"/>
       <c r="H55" s="2"/>
     </row>
-    <row r="56" spans="7:8" ht="78.75" x14ac:dyDescent="1.05">
+    <row r="56" spans="7:8" ht="78.75">
       <c r="G56" s="2"/>
       <c r="H56" s="2"/>
     </row>
-    <row r="57" spans="7:8" ht="78.75" x14ac:dyDescent="1.05">
+    <row r="57" spans="7:8" ht="78.75">
       <c r="G57" s="2"/>
       <c r="H57" s="2"/>
     </row>
-    <row r="58" spans="7:8" ht="78.75" x14ac:dyDescent="1.05">
+    <row r="58" spans="7:8" ht="78.75">
       <c r="G58" s="2"/>
       <c r="H58" s="2"/>
     </row>
-    <row r="59" spans="7:8" ht="78.75" x14ac:dyDescent="1.05">
+    <row r="59" spans="7:8" ht="78.75">
       <c r="G59" s="2"/>
       <c r="H59" s="2"/>
     </row>
-    <row r="60" spans="7:8" ht="78.75" x14ac:dyDescent="1.05">
+    <row r="60" spans="7:8" ht="78.75">
       <c r="G60" s="2"/>
       <c r="H60" s="2"/>
     </row>
-    <row r="61" spans="7:8" ht="78.75" x14ac:dyDescent="1.05">
+    <row r="61" spans="7:8" ht="78.75">
       <c r="G61" s="2"/>
       <c r="H61" s="2"/>
     </row>
-    <row r="62" spans="7:8" ht="78.75" x14ac:dyDescent="1.05">
+    <row r="62" spans="7:8" ht="78.75">
       <c r="G62" s="2"/>
       <c r="H62" s="2"/>
     </row>
-    <row r="63" spans="7:8" ht="78.75" x14ac:dyDescent="1.05">
+    <row r="63" spans="7:8" ht="78.75">
       <c r="G63" s="2"/>
       <c r="H63" s="2"/>
     </row>
-    <row r="64" spans="7:8" ht="78.75" x14ac:dyDescent="1.05">
+    <row r="64" spans="7:8" ht="78.75">
       <c r="G64" s="2"/>
       <c r="H64" s="2"/>
     </row>
-    <row r="65" spans="7:8" ht="78.75" x14ac:dyDescent="1.05">
+    <row r="65" spans="7:8" ht="78.75">
       <c r="G65" s="2"/>
       <c r="H65" s="2"/>
     </row>
-    <row r="66" spans="7:8" ht="78.75" x14ac:dyDescent="1.05">
+    <row r="66" spans="7:8" ht="78.75">
       <c r="G66" s="2"/>
       <c r="H66" s="2"/>
     </row>
-    <row r="67" spans="7:8" ht="78.75" x14ac:dyDescent="1.05">
+    <row r="67" spans="7:8" ht="78.75">
       <c r="G67" s="2"/>
       <c r="H67" s="2"/>
     </row>
-    <row r="68" spans="7:8" ht="78.75" x14ac:dyDescent="1.05">
+    <row r="68" spans="7:8" ht="78.75">
       <c r="G68" s="2"/>
       <c r="H68" s="2"/>
     </row>
-    <row r="69" spans="7:8" ht="78.75" x14ac:dyDescent="1.05">
+    <row r="69" spans="7:8" ht="78.75">
       <c r="G69" s="2"/>
       <c r="H69" s="2"/>
     </row>
-    <row r="70" spans="7:8" ht="78.75" x14ac:dyDescent="1.05">
+    <row r="70" spans="7:8" ht="78.75">
       <c r="G70" s="2"/>
       <c r="H70" s="2"/>
     </row>
-    <row r="71" spans="7:8" ht="78.75" x14ac:dyDescent="1.05">
+    <row r="71" spans="7:8" ht="78.75">
       <c r="G71" s="2"/>
       <c r="H71" s="2"/>
     </row>
-    <row r="72" spans="7:8" ht="78.75" x14ac:dyDescent="1.05">
+    <row r="72" spans="7:8" ht="78.75">
       <c r="G72" s="2"/>
       <c r="H72" s="2"/>
     </row>
-    <row r="73" spans="7:8" ht="78.75" x14ac:dyDescent="1.05">
+    <row r="73" spans="7:8" ht="78.75">
       <c r="G73" s="2"/>
       <c r="H73" s="2"/>
     </row>
-    <row r="74" spans="7:8" ht="78.75" x14ac:dyDescent="1.05">
+    <row r="74" spans="7:8" ht="78.75">
       <c r="G74" s="2"/>
       <c r="H74" s="2"/>
     </row>
-    <row r="75" spans="7:8" ht="78.75" x14ac:dyDescent="1.05">
+    <row r="75" spans="7:8" ht="78.75">
       <c r="G75" s="2"/>
       <c r="H75" s="2"/>
     </row>
-    <row r="76" spans="7:8" ht="78.75" x14ac:dyDescent="1.05">
+    <row r="76" spans="7:8" ht="78.75">
       <c r="G76" s="2"/>
       <c r="H76" s="2"/>
     </row>
-    <row r="77" spans="7:8" ht="78.75" x14ac:dyDescent="1.05">
+    <row r="77" spans="7:8" ht="78.75">
       <c r="G77" s="2"/>
       <c r="H77" s="2"/>
     </row>
-    <row r="78" spans="7:8" ht="78.75" x14ac:dyDescent="1.05">
+    <row r="78" spans="7:8" ht="78.75">
       <c r="G78" s="2"/>
       <c r="H78" s="2"/>
     </row>
-    <row r="79" spans="7:8" ht="78.75" x14ac:dyDescent="1.05">
+    <row r="79" spans="7:8" ht="78.75">
       <c r="G79" s="2"/>
       <c r="H79" s="2"/>
     </row>
-    <row r="80" spans="7:8" ht="78.75" x14ac:dyDescent="1.05">
+    <row r="80" spans="7:8" ht="78.75">
       <c r="G80" s="2"/>
       <c r="H80" s="2"/>
     </row>
-    <row r="81" spans="7:8" ht="78.75" x14ac:dyDescent="1.05">
+    <row r="81" spans="7:8" ht="78.75">
       <c r="G81" s="2"/>
       <c r="H81" s="2"/>
     </row>
-    <row r="82" spans="7:8" ht="78.75" x14ac:dyDescent="1.05">
+    <row r="82" spans="7:8" ht="78.75">
       <c r="G82" s="2"/>
       <c r="H82" s="2"/>
     </row>
-    <row r="83" spans="7:8" ht="78.75" x14ac:dyDescent="1.05">
+    <row r="83" spans="7:8" ht="78.75">
       <c r="G83" s="2"/>
       <c r="H83" s="2"/>
     </row>
-    <row r="84" spans="7:8" ht="78.75" x14ac:dyDescent="1.05">
+    <row r="84" spans="7:8" ht="78.75">
       <c r="G84" s="2"/>
       <c r="H84" s="2"/>
     </row>
-    <row r="85" spans="7:8" ht="78.75" x14ac:dyDescent="1.05">
+    <row r="85" spans="7:8" ht="78.75">
       <c r="G85" s="2"/>
       <c r="H85" s="2"/>
     </row>
-    <row r="86" spans="7:8" ht="78.75" x14ac:dyDescent="1.05">
+    <row r="86" spans="7:8" ht="78.75">
       <c r="G86" s="2"/>
       <c r="H86" s="2"/>
     </row>
-    <row r="87" spans="7:8" ht="78.75" x14ac:dyDescent="1.05">
+    <row r="87" spans="7:8" ht="78.75">
       <c r="G87" s="2"/>
       <c r="H87" s="2"/>
     </row>
-    <row r="88" spans="7:8" ht="78.75" x14ac:dyDescent="1.05">
+    <row r="88" spans="7:8" ht="78.75">
       <c r="G88" s="2"/>
       <c r="H88" s="2"/>
     </row>
-    <row r="89" spans="7:8" ht="78.75" x14ac:dyDescent="1.05">
+    <row r="89" spans="7:8" ht="78.75">
       <c r="G89" s="2"/>
       <c r="H89" s="2"/>
     </row>
-    <row r="90" spans="7:8" ht="78.75" x14ac:dyDescent="1.05">
+    <row r="90" spans="7:8" ht="78.75">
       <c r="G90" s="2"/>
       <c r="H90" s="2"/>
     </row>
-    <row r="91" spans="7:8" ht="78.75" x14ac:dyDescent="1.05">
+    <row r="91" spans="7:8" ht="78.75">
       <c r="G91" s="2"/>
       <c r="H91" s="2"/>
     </row>

</xml_diff>